<commit_message>
Pictures for upcoming event
</commit_message>
<xml_diff>
--- a/Budget2022.xlsx
+++ b/Budget2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rakul/Desktop/SWU/lillekat.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46E948B-EA94-4F43-A071-AFD0413AE121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81870118-63F4-2E4F-B0A5-FDE2B9BE6D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25520" windowHeight="14900" xr2:uid="{D1CCE3FA-2749-BB47-B79F-67BB4C56A698}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>Lillekat 2022 budget</t>
   </si>
@@ -81,10 +81,16 @@
     <t>I alt</t>
   </si>
   <si>
-    <t>Til faktura</t>
-  </si>
-  <si>
     <t>Levering</t>
+  </si>
+  <si>
+    <t>6+CF</t>
+  </si>
+  <si>
+    <t>Pris</t>
+  </si>
+  <si>
+    <t>Sum</t>
   </si>
 </sst>
 </file>
@@ -140,7 +146,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -295,11 +301,96 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -338,6 +429,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -652,16 +762,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F117A488-0249-9540-9962-645D5D55DAA6}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
@@ -692,7 +802,7 @@
       <c r="G2" s="25"/>
       <c r="H2" s="25"/>
     </row>
-    <row r="3" spans="1:8" ht="28" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="31" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -712,7 +822,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H3" s="19" t="s">
         <v>4</v>
@@ -868,14 +978,150 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="28"/>
+      <c r="D11" s="26" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
-        <v>15</v>
-      </c>
-    </row>
+      <c r="A12" s="23"/>
+      <c r="B12" s="29">
+        <v>1</v>
+      </c>
+      <c r="C12" s="30">
+        <v>1</v>
+      </c>
+      <c r="D12" s="31">
+        <f>95*B12</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="29">
+        <v>1</v>
+      </c>
+      <c r="C13" s="30">
+        <v>2</v>
+      </c>
+      <c r="D13" s="31">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="29">
+        <v>1</v>
+      </c>
+      <c r="C14" s="30">
+        <v>4</v>
+      </c>
+      <c r="D14" s="31">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="29">
+        <v>2</v>
+      </c>
+      <c r="C15" s="30">
+        <v>5</v>
+      </c>
+      <c r="D15" s="31">
+        <f>130*B15</f>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="29">
+        <v>1</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="31">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="29">
+        <v>2</v>
+      </c>
+      <c r="C17" s="30">
+        <v>10</v>
+      </c>
+      <c r="D17" s="31">
+        <f>105*B17</f>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="29">
+        <v>1</v>
+      </c>
+      <c r="C18" s="30">
+        <v>12</v>
+      </c>
+      <c r="D18" s="31">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="29">
+        <v>2</v>
+      </c>
+      <c r="C19" s="30">
+        <v>13</v>
+      </c>
+      <c r="D19" s="31">
+        <f>110*B19</f>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="29">
+        <v>2</v>
+      </c>
+      <c r="C20" s="30">
+        <v>24</v>
+      </c>
+      <c r="D20" s="31">
+        <f>130*B20</f>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="33">
+        <v>1</v>
+      </c>
+      <c r="C21" s="34">
+        <v>29</v>
+      </c>
+      <c r="D21" s="35">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="36">
+        <f>SUM(B12:B21)</f>
+        <v>14</v>
+      </c>
+      <c r="C22" s="37"/>
+      <c r="D22" s="38">
+        <f>SUM(D12:D21)</f>
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:H2"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>